<commit_message>
Add open account test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -214,7 +214,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -323,10 +323,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
@@ -338,9 +338,7 @@
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -349,9 +347,7 @@
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C2" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -375,7 +371,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Add runmodes for test suites
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="OpenAccountTest" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="test_suite" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="testSuite" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -63,7 +63,7 @@
     <t xml:space="preserve">Alvez</t>
   </si>
   <si>
-    <t xml:space="preserve">N</t>
+    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">Jorge</t>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
   </si>
   <si>
     <t xml:space="preserve">TCID</t>
@@ -211,10 +214,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -323,10 +326,10 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
@@ -338,7 +341,9 @@
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -347,7 +352,9 @@
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -368,41 +375,41 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add runmodes for test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -72,6 +72,9 @@
     <t xml:space="preserve">Souza</t>
   </si>
   <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
     <t xml:space="preserve">customer</t>
   </si>
   <si>
@@ -84,13 +87,7 @@
     <t xml:space="preserve">Dollar</t>
   </si>
   <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Runmode</t>
+    <t xml:space="preserve">tcid</t>
   </si>
   <si>
     <t xml:space="preserve">BankManagerLoginTest</t>
@@ -213,11 +210,11 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -304,7 +301,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -325,21 +322,21 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -347,13 +344,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -375,22 +372,22 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
@@ -398,7 +395,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -406,10 +403,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improves parameterization using hashtable
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t xml:space="preserve">Souza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
   </si>
   <si>
     <t xml:space="preserve">customer</t>
@@ -210,11 +207,11 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -301,7 +298,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -323,20 +320,20 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -344,13 +341,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -371,15 +368,15 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -387,7 +384,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
@@ -395,7 +392,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -403,10 +400,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvements to TestBase class
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -57,31 +57,19 @@
     <t xml:space="preserve">Santos</t>
   </si>
   <si>
-    <t xml:space="preserve">Jose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alvez</t>
+    <t xml:space="preserve">customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joao Silva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dollar</t>
   </si>
   <si>
     <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jorge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Souza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">customer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">currency</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joao Silva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dollar</t>
   </si>
   <si>
     <t xml:space="preserve">tcid</t>
@@ -205,13 +193,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -265,40 +253,6 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>123654</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>789456</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -323,17 +277,17 @@
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -341,13 +295,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -372,11 +326,11 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
@@ -384,26 +338,26 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improves extent reports and console output
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">Customer added successfully</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
+    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">Maria</t>
@@ -57,6 +57,9 @@
     <t xml:space="preserve">Santos</t>
   </si>
   <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
     <t xml:space="preserve">customer</t>
   </si>
   <si>
@@ -67,9 +70,6 @@
   </si>
   <si>
     <t xml:space="preserve">Dollar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">tcid</t>
@@ -195,11 +195,11 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -252,7 +252,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -277,17 +277,17 @@
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -295,13 +295,13 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -322,11 +322,11 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -341,7 +341,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -349,7 +349,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,7 +357,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor open account test using page objects model
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -66,7 +66,7 @@
     <t xml:space="preserve">currency</t>
   </si>
   <si>
-    <t xml:space="preserve">Joao Silva</t>
+    <t xml:space="preserve">Harry Potter</t>
   </si>
   <si>
     <t xml:space="preserve">Dollar</t>
@@ -195,11 +195,11 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -258,7 +258,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -273,11 +273,11 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
@@ -307,7 +307,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -326,7 +326,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -363,7 +363,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Refactor open account test using page objects model (#2)
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -66,7 +66,7 @@
     <t xml:space="preserve">currency</t>
   </si>
   <si>
-    <t xml:space="preserve">Joao Silva</t>
+    <t xml:space="preserve">Harry Potter</t>
   </si>
   <si>
     <t xml:space="preserve">Dollar</t>
@@ -195,11 +195,11 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -258,7 +258,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -273,11 +273,11 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
@@ -307,7 +307,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -326,7 +326,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -363,7 +363,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Add table utils methods
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -199,7 +199,7 @@
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
   </cols>
@@ -273,11 +273,11 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.59"/>
   </cols>
@@ -322,11 +322,11 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -349,7 +349,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>